<commit_message>
xlsx: support for generating dynamic cells in a loop, support for preserving rich text in cell, support for setting explicit cell type and fix concat tags
we now support generating cells both horizontally and vertically in single loop.

`each` helper now supports new parameter `cells` to specify that user wants to generate/expand cells dynamically in both directions (horizontally and vertically)

the `cells` value is expected to be an array, each item should be another array that contains the values to generate. if you have an input like this `[['One', 'Two'], ['Three', 'Four', 'Five']]` then the loop will generate 2 rows, the first row will contain 2 cells, and the second row will contain 3 cells.
- concat tags now works correctly, previously it was searching for w:t nodes but in xlsx the nodes are just t
- add new helper `xlsxCType` to set explicit cell type, useful when there is dynamic content and we can not use the auto-detect anymore
</commit_message>
<xml_diff>
--- a/packages/jsreport-xlsx/test/xlsx/loop-left-preserve.xlsx
+++ b/packages/jsreport-xlsx/test/xlsx/loop-left-preserve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/jsreport/jsreport/packages/jsreport-xlsx/test/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84AD373-16F3-0A44-B700-0D2E98966707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D399F639-B33A-8441-B862-0801530DF877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="2880" windowWidth="28040" windowHeight="17440" xr2:uid="{E64D1ECD-F10D-4745-832B-F27334D20F18}"/>
+    <workbookView xWindow="8360" yWindow="2580" windowWidth="28040" windowHeight="17440" xr2:uid="{E64D1ECD-F10D-4745-832B-F27334D20F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,7 +412,7 @@
   <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>